<commit_message>
debugging tables and design
</commit_message>
<xml_diff>
--- a/reports/overall_expenses.xlsx
+++ b/reports/overall_expenses.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
   <si>
     <t>No.</t>
   </si>
@@ -227,9 +227,6 @@
     <t>1,486.00</t>
   </si>
   <si>
-    <t>ALASKA CREAMY CHICKEN EVAP 250ML</t>
-  </si>
-  <si>
     <t>PURCHASED ORDER</t>
   </si>
   <si>
@@ -239,10 +236,31 @@
     <t>10-000000106</t>
   </si>
   <si>
+    <t>CLOUD 9</t>
+  </si>
+  <si>
+    <t>Jun 25, 2024</t>
+  </si>
+  <si>
+    <t>Pieces</t>
+  </si>
+  <si>
+    <t>10-000000001</t>
+  </si>
+  <si>
+    <t>10,000.00</t>
+  </si>
+  <si>
+    <t>555 TUNA SPICY PAKSIW</t>
+  </si>
+  <si>
+    <t>30,000.00</t>
+  </si>
+  <si>
     <t>Total Expenses</t>
   </si>
   <si>
-    <t>816,831.66</t>
+    <t>856,831.66</t>
   </si>
 </sst>
 </file>
@@ -621,16 +639,16 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:L25"/>
+      <selection activeCell="A1" sqref="A1:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="6.856" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="41.133" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="28.136" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="25.708" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="32.849" bestFit="true" customWidth="true" style="0"/>
@@ -1485,27 +1503,25 @@
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F24" s="2">
         <v>25</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>47</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J24" s="2">
         <v>36.45</v>
@@ -1518,26 +1534,98 @@
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="2">
+        <v>50</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J25" s="2">
+        <v>200.0</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.0</v>
+      </c>
       <c r="L25" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" s="2">
+        <v>200</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>75</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J26" s="2">
+        <v>150.0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="A27:K27"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>